<commit_message>
feat: Enhance admin management and document handling
- Updated User interface to include optional fields for admin contact details.
- Implemented logic to ensure exactly two default admin accounts are created.
- Added validation to restrict admin role changes and deletions to maintain admin count.
- Improved error handling and user feedback for assignment updates in document management.
- Enhanced API for AOI tables to support optional user filtering.
- Updated Vite configuration for improved development experience.
- Modified output Excel file to reflect recent changes.
</commit_message>
<xml_diff>
--- a/web-output/output.xlsx
+++ b/web-output/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="104">
   <si>
     <t>Level</t>
   </si>
@@ -58,15 +58,24 @@
     <t>Export_Date</t>
   </si>
   <si>
+    <t>Jenis_Penilaian</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>header</t>
   </si>
   <si>
     <t>total</t>
   </si>
   <si>
+    <t>indicator</t>
+  </si>
+  <si>
     <t>I</t>
   </si>
   <si>
@@ -88,6 +97,9 @@
     <t>TOTAL</t>
   </si>
   <si>
+    <t>Test Aspect</t>
+  </si>
+  <si>
     <t>brief-2014-I-0</t>
   </si>
   <si>
@@ -106,22 +118,148 @@
     <t>brief-2014-VI-5</t>
   </si>
   <si>
-    <t>predetermined-1756694617975-0</t>
-  </si>
-  <si>
-    <t>predetermined-1756694625933-1</t>
-  </si>
-  <si>
-    <t>predetermined-1756694631505-2</t>
-  </si>
-  <si>
-    <t>predetermined-1756694638616-3</t>
-  </si>
-  <si>
-    <t>predetermined-1756694645111-4</t>
-  </si>
-  <si>
-    <t>predetermined-1756694649498-5</t>
+    <t>brief-2015-I-0</t>
+  </si>
+  <si>
+    <t>brief-2015-II-1</t>
+  </si>
+  <si>
+    <t>brief-2015-III-2</t>
+  </si>
+  <si>
+    <t>brief-2015-IV-3</t>
+  </si>
+  <si>
+    <t>brief-2015-V-4</t>
+  </si>
+  <si>
+    <t>brief-2015-VI-5</t>
+  </si>
+  <si>
+    <t>brief-2016-I-0</t>
+  </si>
+  <si>
+    <t>brief-2016-II-1</t>
+  </si>
+  <si>
+    <t>brief-2016-III-2</t>
+  </si>
+  <si>
+    <t>brief-2016-IV-3</t>
+  </si>
+  <si>
+    <t>brief-2016-V-4</t>
+  </si>
+  <si>
+    <t>brief-2016-VI-5</t>
+  </si>
+  <si>
+    <t>predetermined-1758260064005-0</t>
+  </si>
+  <si>
+    <t>predetermined-1758260065869-1</t>
+  </si>
+  <si>
+    <t>predetermined-1758260067857-2</t>
+  </si>
+  <si>
+    <t>predetermined-1758260069936-3</t>
+  </si>
+  <si>
+    <t>predetermined-1758260072187-4</t>
+  </si>
+  <si>
+    <t>predetermined-1758260075756-5</t>
+  </si>
+  <si>
+    <t>brief-2018-I-0</t>
+  </si>
+  <si>
+    <t>brief-2018-II-1</t>
+  </si>
+  <si>
+    <t>brief-2018-III-2</t>
+  </si>
+  <si>
+    <t>brief-2018-IV-3</t>
+  </si>
+  <si>
+    <t>brief-2018-V-4</t>
+  </si>
+  <si>
+    <t>brief-2018-VI-5</t>
+  </si>
+  <si>
+    <t>predetermined-1758260012501-0</t>
+  </si>
+  <si>
+    <t>predetermined-1758260015089-1</t>
+  </si>
+  <si>
+    <t>predetermined-1758260017189-2</t>
+  </si>
+  <si>
+    <t>predetermined-1758260019225-3</t>
+  </si>
+  <si>
+    <t>predetermined-1758260021157-4</t>
+  </si>
+  <si>
+    <t>predetermined-1758260023298-5</t>
+  </si>
+  <si>
+    <t>predetermined-1758259989336-0</t>
+  </si>
+  <si>
+    <t>predetermined-1758259991690-1</t>
+  </si>
+  <si>
+    <t>predetermined-1758259994007-2</t>
+  </si>
+  <si>
+    <t>predetermined-1758259996408-3</t>
+  </si>
+  <si>
+    <t>predetermined-1758259998662-4</t>
+  </si>
+  <si>
+    <t>predetermined-1758260000617-5</t>
+  </si>
+  <si>
+    <t>predetermined-1758259959678-0</t>
+  </si>
+  <si>
+    <t>predetermined-1758259961998-1</t>
+  </si>
+  <si>
+    <t>predetermined-1758259963966-2</t>
+  </si>
+  <si>
+    <t>predetermined-1758259965611-3</t>
+  </si>
+  <si>
+    <t>predetermined-1758259967615-4</t>
+  </si>
+  <si>
+    <t>predetermined-1758259969552-5</t>
+  </si>
+  <si>
+    <t>predetermined-1758259909317-0</t>
+  </si>
+  <si>
+    <t>predetermined-1758259912833-1</t>
+  </si>
+  <si>
+    <t>predetermined-1758259914872-2</t>
+  </si>
+  <si>
+    <t>predetermined-1758259917387-3</t>
+  </si>
+  <si>
+    <t>predetermined-1758259922924-4</t>
+  </si>
+  <si>
+    <t>predetermined-1758259925592-5</t>
   </si>
   <si>
     <t>Komitmen terhadap Penerapan Tata Kelola secara Berkelanjutan</t>
@@ -142,6 +280,18 @@
     <t>Aspek Lainnya</t>
   </si>
   <si>
+    <t>Komitmen Terhadap Penerapan Tata Kelola Perusahaan yang Baik Secara Berkelanjutan</t>
+  </si>
+  <si>
+    <t>Pemegang Saham dan RUPS/Pemilik Modal</t>
+  </si>
+  <si>
+    <t>Dewan Komisaris/Dewan Pengawas</t>
+  </si>
+  <si>
+    <t>Test assessment description</t>
+  </si>
+  <si>
     <t>Baik</t>
   </si>
   <si>
@@ -154,7 +304,28 @@
     <t>Tidak Baik</t>
   </si>
   <si>
-    <t>2025-09-02</t>
+    <t>BPKP Provinsi Jawa Barat</t>
+  </si>
+  <si>
+    <t>PT Bumi Pertiwi Mandiri + PPA&amp;K</t>
+  </si>
+  <si>
+    <t>PT Management Indonesia Mandiri</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>2025-09-19</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Internal</t>
   </si>
 </sst>
 </file>
@@ -512,13 +683,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,25 +732,25 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2">
-        <v>1</v>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -591,33 +762,36 @@
         <v>83</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="K2">
         <v>2014</v>
       </c>
+      <c r="L2" t="s">
+        <v>96</v>
+      </c>
       <c r="N2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="O2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G3">
         <v>9</v>
@@ -629,33 +803,36 @@
         <v>93</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K3">
         <v>2014</v>
       </c>
+      <c r="L3" t="s">
+        <v>96</v>
+      </c>
       <c r="N3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="O3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="G4">
         <v>35</v>
@@ -667,33 +844,36 @@
         <v>90</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K4">
         <v>2014</v>
       </c>
+      <c r="L4" t="s">
+        <v>96</v>
+      </c>
       <c r="N4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="O4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G5">
         <v>35</v>
@@ -705,33 +885,36 @@
         <v>87</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K5">
         <v>2014</v>
       </c>
+      <c r="L5" t="s">
+        <v>96</v>
+      </c>
       <c r="N5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="O5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="G6">
         <v>9</v>
@@ -743,33 +926,36 @@
         <v>72</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="K6">
         <v>2014</v>
       </c>
+      <c r="L6" t="s">
+        <v>96</v>
+      </c>
       <c r="N6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="O6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -781,68 +967,74 @@
         <v>-20</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="K7">
         <v>2014</v>
       </c>
+      <c r="L7" t="s">
+        <v>96</v>
+      </c>
       <c r="N7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="O7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G8">
         <v>100</v>
       </c>
       <c r="H8">
-        <v>83.617</v>
+        <v>81.79300000000001</v>
       </c>
       <c r="I8">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="K8">
         <v>2014</v>
       </c>
+      <c r="L8" t="s">
+        <v>96</v>
+      </c>
       <c r="N8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="G9">
         <v>7</v>
@@ -854,33 +1046,33 @@
         <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K9">
         <v>2015</v>
       </c>
       <c r="N9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G10">
         <v>9</v>
@@ -892,33 +1084,33 @@
         <v>90</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K10">
         <v>2015</v>
       </c>
       <c r="N10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>35</v>
@@ -930,33 +1122,33 @@
         <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K11">
         <v>2015</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12">
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G12">
         <v>35</v>
@@ -968,33 +1160,33 @@
         <v>88</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K12">
         <v>2015</v>
       </c>
       <c r="N12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13">
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="G13">
         <v>9</v>
@@ -1006,33 +1198,33 @@
         <v>86</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K13">
         <v>2015</v>
       </c>
       <c r="N13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14">
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -1044,30 +1236,30 @@
         <v>-20</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="K14">
         <v>2015</v>
       </c>
       <c r="N14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>14</v>
+        <v>100</v>
+      </c>
+      <c r="O14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15">
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -1079,13 +1271,1980 @@
         <v>85</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K15">
         <v>2015</v>
       </c>
       <c r="N15" t="s">
+        <v>100</v>
+      </c>
+      <c r="O15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>6.189</v>
+      </c>
+      <c r="I16">
+        <v>88</v>
+      </c>
+      <c r="J16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16">
+        <v>2016</v>
+      </c>
+      <c r="L16" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" t="s">
+        <v>100</v>
+      </c>
+      <c r="O16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>8.553000000000001</v>
+      </c>
+      <c r="I17">
+        <v>95</v>
+      </c>
+      <c r="J17" t="s">
+        <v>93</v>
+      </c>
+      <c r="K17">
+        <v>2016</v>
+      </c>
+      <c r="L17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N17" t="s">
+        <v>100</v>
+      </c>
+      <c r="O17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18">
+        <v>35</v>
+      </c>
+      <c r="H18">
+        <v>31.857</v>
+      </c>
+      <c r="I18">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18">
+        <v>2016</v>
+      </c>
+      <c r="L18" t="s">
+        <v>96</v>
+      </c>
+      <c r="N18" t="s">
+        <v>100</v>
+      </c>
+      <c r="O18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19">
+        <v>35</v>
+      </c>
+      <c r="H19">
+        <v>31.485</v>
+      </c>
+      <c r="I19">
+        <v>90</v>
+      </c>
+      <c r="J19" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19">
+        <v>2016</v>
+      </c>
+      <c r="L19" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" t="s">
+        <v>100</v>
+      </c>
+      <c r="O19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <v>7.272</v>
+      </c>
+      <c r="I20">
+        <v>81</v>
+      </c>
+      <c r="J20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20">
+        <v>2016</v>
+      </c>
+      <c r="L20" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" t="s">
+        <v>100</v>
+      </c>
+      <c r="O20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>95</v>
+      </c>
+      <c r="K21">
+        <v>2016</v>
+      </c>
+      <c r="L21" t="s">
+        <v>96</v>
+      </c>
+      <c r="N21" t="s">
+        <v>100</v>
+      </c>
+      <c r="O21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>85.35599999999999</v>
+      </c>
+      <c r="I22">
+        <v>85</v>
+      </c>
+      <c r="J22" t="s">
+        <v>93</v>
+      </c>
+      <c r="K22">
+        <v>2016</v>
+      </c>
+      <c r="L22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" t="s">
+        <v>100</v>
+      </c>
+      <c r="O22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
         <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>6.6259</v>
+      </c>
+      <c r="I23">
+        <v>95</v>
+      </c>
+      <c r="J23" t="s">
+        <v>93</v>
+      </c>
+      <c r="K23">
+        <v>2017</v>
+      </c>
+      <c r="N23" t="s">
+        <v>100</v>
+      </c>
+      <c r="O23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
+      </c>
+      <c r="H24">
+        <v>8.5526</v>
+      </c>
+      <c r="I24">
+        <v>95</v>
+      </c>
+      <c r="J24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24">
+        <v>2017</v>
+      </c>
+      <c r="N24" t="s">
+        <v>100</v>
+      </c>
+      <c r="O24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25">
+        <v>35</v>
+      </c>
+      <c r="H25">
+        <v>31.8687</v>
+      </c>
+      <c r="I25">
+        <v>91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25">
+        <v>2017</v>
+      </c>
+      <c r="N25" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26">
+        <v>35</v>
+      </c>
+      <c r="H26">
+        <v>31.4548</v>
+      </c>
+      <c r="I26">
+        <v>90</v>
+      </c>
+      <c r="J26" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26">
+        <v>2017</v>
+      </c>
+      <c r="N26" t="s">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>7.9498</v>
+      </c>
+      <c r="I27">
+        <v>88</v>
+      </c>
+      <c r="J27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K27">
+        <v>2017</v>
+      </c>
+      <c r="N27" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>20</v>
+      </c>
+      <c r="J28" t="s">
+        <v>95</v>
+      </c>
+      <c r="K28">
+        <v>2017</v>
+      </c>
+      <c r="N28" t="s">
+        <v>100</v>
+      </c>
+      <c r="O28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>87.4517</v>
+      </c>
+      <c r="I29">
+        <v>87</v>
+      </c>
+      <c r="J29" t="s">
+        <v>93</v>
+      </c>
+      <c r="K29">
+        <v>2017</v>
+      </c>
+      <c r="N29" t="s">
+        <v>100</v>
+      </c>
+      <c r="O29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>6.291</v>
+      </c>
+      <c r="I30">
+        <v>90</v>
+      </c>
+      <c r="J30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K30">
+        <v>2018</v>
+      </c>
+      <c r="L30" t="s">
+        <v>96</v>
+      </c>
+      <c r="N30" t="s">
+        <v>100</v>
+      </c>
+      <c r="O30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>8.225</v>
+      </c>
+      <c r="I31">
+        <v>91</v>
+      </c>
+      <c r="J31" t="s">
+        <v>93</v>
+      </c>
+      <c r="K31">
+        <v>2018</v>
+      </c>
+      <c r="L31" t="s">
+        <v>96</v>
+      </c>
+      <c r="N31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32">
+        <v>35</v>
+      </c>
+      <c r="H32">
+        <v>32.339</v>
+      </c>
+      <c r="I32">
+        <v>92</v>
+      </c>
+      <c r="J32" t="s">
+        <v>93</v>
+      </c>
+      <c r="K32">
+        <v>2018</v>
+      </c>
+      <c r="L32" t="s">
+        <v>96</v>
+      </c>
+      <c r="N32" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33">
+        <v>35</v>
+      </c>
+      <c r="H33">
+        <v>30.989</v>
+      </c>
+      <c r="I33">
+        <v>89</v>
+      </c>
+      <c r="J33" t="s">
+        <v>93</v>
+      </c>
+      <c r="K33">
+        <v>2018</v>
+      </c>
+      <c r="L33" t="s">
+        <v>96</v>
+      </c>
+      <c r="N33" t="s">
+        <v>100</v>
+      </c>
+      <c r="O33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>7.709</v>
+      </c>
+      <c r="I34">
+        <v>86</v>
+      </c>
+      <c r="J34" t="s">
+        <v>93</v>
+      </c>
+      <c r="K34">
+        <v>2018</v>
+      </c>
+      <c r="L34" t="s">
+        <v>96</v>
+      </c>
+      <c r="N34" t="s">
+        <v>100</v>
+      </c>
+      <c r="O34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>-1</v>
+      </c>
+      <c r="I35">
+        <v>-20</v>
+      </c>
+      <c r="J35" t="s">
+        <v>95</v>
+      </c>
+      <c r="K35">
+        <v>2018</v>
+      </c>
+      <c r="L35" t="s">
+        <v>96</v>
+      </c>
+      <c r="N35" t="s">
+        <v>100</v>
+      </c>
+      <c r="O35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36">
+        <v>100</v>
+      </c>
+      <c r="H36">
+        <v>84.553</v>
+      </c>
+      <c r="I36">
+        <v>85</v>
+      </c>
+      <c r="J36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K36">
+        <v>2018</v>
+      </c>
+      <c r="L36" t="s">
+        <v>96</v>
+      </c>
+      <c r="N36" t="s">
+        <v>100</v>
+      </c>
+      <c r="O36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37">
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <v>6.17</v>
+      </c>
+      <c r="I37">
+        <v>88</v>
+      </c>
+      <c r="J37" t="s">
+        <v>93</v>
+      </c>
+      <c r="K37">
+        <v>2019</v>
+      </c>
+      <c r="L37" t="s">
+        <v>97</v>
+      </c>
+      <c r="N37" t="s">
+        <v>100</v>
+      </c>
+      <c r="O37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>8.82</v>
+      </c>
+      <c r="I38">
+        <v>98</v>
+      </c>
+      <c r="J38" t="s">
+        <v>93</v>
+      </c>
+      <c r="K38">
+        <v>2019</v>
+      </c>
+      <c r="L38" t="s">
+        <v>97</v>
+      </c>
+      <c r="N38" t="s">
+        <v>100</v>
+      </c>
+      <c r="O38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39">
+        <v>35</v>
+      </c>
+      <c r="H39">
+        <v>33.179</v>
+      </c>
+      <c r="I39">
+        <v>95</v>
+      </c>
+      <c r="J39" t="s">
+        <v>93</v>
+      </c>
+      <c r="K39">
+        <v>2019</v>
+      </c>
+      <c r="L39" t="s">
+        <v>97</v>
+      </c>
+      <c r="N39" t="s">
+        <v>100</v>
+      </c>
+      <c r="O39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40">
+        <v>35</v>
+      </c>
+      <c r="H40">
+        <v>32.302</v>
+      </c>
+      <c r="I40">
+        <v>92</v>
+      </c>
+      <c r="J40" t="s">
+        <v>93</v>
+      </c>
+      <c r="K40">
+        <v>2019</v>
+      </c>
+      <c r="L40" t="s">
+        <v>97</v>
+      </c>
+      <c r="N40" t="s">
+        <v>100</v>
+      </c>
+      <c r="O40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41">
+        <v>9</v>
+      </c>
+      <c r="H41">
+        <v>7.674</v>
+      </c>
+      <c r="I41">
+        <v>85</v>
+      </c>
+      <c r="J41" t="s">
+        <v>93</v>
+      </c>
+      <c r="K41">
+        <v>2019</v>
+      </c>
+      <c r="L41" t="s">
+        <v>97</v>
+      </c>
+      <c r="N41" t="s">
+        <v>100</v>
+      </c>
+      <c r="O41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <v>0.625</v>
+      </c>
+      <c r="I42">
+        <v>13</v>
+      </c>
+      <c r="J42" t="s">
+        <v>95</v>
+      </c>
+      <c r="K42">
+        <v>2019</v>
+      </c>
+      <c r="L42" t="s">
+        <v>97</v>
+      </c>
+      <c r="N42" t="s">
+        <v>100</v>
+      </c>
+      <c r="O42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43">
+        <v>100</v>
+      </c>
+      <c r="H43">
+        <v>88.76900000000001</v>
+      </c>
+      <c r="I43">
+        <v>89</v>
+      </c>
+      <c r="J43" t="s">
+        <v>93</v>
+      </c>
+      <c r="K43">
+        <v>2019</v>
+      </c>
+      <c r="L43" t="s">
+        <v>97</v>
+      </c>
+      <c r="N43" t="s">
+        <v>100</v>
+      </c>
+      <c r="O43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44">
+        <v>6.328</v>
+      </c>
+      <c r="I44">
+        <v>90</v>
+      </c>
+      <c r="J44" t="s">
+        <v>93</v>
+      </c>
+      <c r="K44">
+        <v>2020</v>
+      </c>
+      <c r="L44" t="s">
+        <v>96</v>
+      </c>
+      <c r="N44" t="s">
+        <v>100</v>
+      </c>
+      <c r="O44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45">
+        <v>9</v>
+      </c>
+      <c r="H45">
+        <v>8.423</v>
+      </c>
+      <c r="I45">
+        <v>94</v>
+      </c>
+      <c r="J45" t="s">
+        <v>93</v>
+      </c>
+      <c r="K45">
+        <v>2020</v>
+      </c>
+      <c r="L45" t="s">
+        <v>96</v>
+      </c>
+      <c r="N45" t="s">
+        <v>100</v>
+      </c>
+      <c r="O45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46">
+        <v>35</v>
+      </c>
+      <c r="H46">
+        <v>33.421</v>
+      </c>
+      <c r="I46">
+        <v>95</v>
+      </c>
+      <c r="J46" t="s">
+        <v>93</v>
+      </c>
+      <c r="K46">
+        <v>2020</v>
+      </c>
+      <c r="L46" t="s">
+        <v>96</v>
+      </c>
+      <c r="N46" t="s">
+        <v>100</v>
+      </c>
+      <c r="O46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47">
+        <v>35</v>
+      </c>
+      <c r="H47">
+        <v>29.677</v>
+      </c>
+      <c r="I47">
+        <v>85</v>
+      </c>
+      <c r="J47" t="s">
+        <v>92</v>
+      </c>
+      <c r="K47">
+        <v>2020</v>
+      </c>
+      <c r="L47" t="s">
+        <v>96</v>
+      </c>
+      <c r="N47" t="s">
+        <v>100</v>
+      </c>
+      <c r="O47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" t="s">
+        <v>86</v>
+      </c>
+      <c r="G48">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <v>7.612</v>
+      </c>
+      <c r="I48">
+        <v>85</v>
+      </c>
+      <c r="J48" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48">
+        <v>2020</v>
+      </c>
+      <c r="L48" t="s">
+        <v>96</v>
+      </c>
+      <c r="N48" t="s">
+        <v>100</v>
+      </c>
+      <c r="O48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>95</v>
+      </c>
+      <c r="K49">
+        <v>2020</v>
+      </c>
+      <c r="L49" t="s">
+        <v>96</v>
+      </c>
+      <c r="N49" t="s">
+        <v>100</v>
+      </c>
+      <c r="O49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" t="s">
+        <v>88</v>
+      </c>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50">
+        <v>6.366</v>
+      </c>
+      <c r="I50">
+        <v>91</v>
+      </c>
+      <c r="J50" t="s">
+        <v>93</v>
+      </c>
+      <c r="K50">
+        <v>2022</v>
+      </c>
+      <c r="L50" t="s">
+        <v>96</v>
+      </c>
+      <c r="N50" t="s">
+        <v>100</v>
+      </c>
+      <c r="O50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51">
+        <v>9</v>
+      </c>
+      <c r="H51">
+        <v>8.243</v>
+      </c>
+      <c r="I51">
+        <v>92</v>
+      </c>
+      <c r="J51" t="s">
+        <v>93</v>
+      </c>
+      <c r="K51">
+        <v>2022</v>
+      </c>
+      <c r="L51" t="s">
+        <v>96</v>
+      </c>
+      <c r="N51" t="s">
+        <v>100</v>
+      </c>
+      <c r="O51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G52">
+        <v>35</v>
+      </c>
+      <c r="H52">
+        <v>32.561</v>
+      </c>
+      <c r="I52">
+        <v>93</v>
+      </c>
+      <c r="J52" t="s">
+        <v>93</v>
+      </c>
+      <c r="K52">
+        <v>2022</v>
+      </c>
+      <c r="L52" t="s">
+        <v>96</v>
+      </c>
+      <c r="N52" t="s">
+        <v>100</v>
+      </c>
+      <c r="O52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" t="s">
+        <v>85</v>
+      </c>
+      <c r="G53">
+        <v>35</v>
+      </c>
+      <c r="H53">
+        <v>30.875</v>
+      </c>
+      <c r="I53">
+        <v>88</v>
+      </c>
+      <c r="J53" t="s">
+        <v>93</v>
+      </c>
+      <c r="K53">
+        <v>2022</v>
+      </c>
+      <c r="L53" t="s">
+        <v>96</v>
+      </c>
+      <c r="N53" t="s">
+        <v>100</v>
+      </c>
+      <c r="O53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>86</v>
+      </c>
+      <c r="G54">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <v>7.187</v>
+      </c>
+      <c r="I54">
+        <v>80</v>
+      </c>
+      <c r="J54" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54">
+        <v>2022</v>
+      </c>
+      <c r="L54" t="s">
+        <v>96</v>
+      </c>
+      <c r="N54" t="s">
+        <v>100</v>
+      </c>
+      <c r="O54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>95</v>
+      </c>
+      <c r="K55">
+        <v>2022</v>
+      </c>
+      <c r="L55" t="s">
+        <v>96</v>
+      </c>
+      <c r="N55" t="s">
+        <v>100</v>
+      </c>
+      <c r="O55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>85.232</v>
+      </c>
+      <c r="I56">
+        <v>85</v>
+      </c>
+      <c r="J56" t="s">
+        <v>93</v>
+      </c>
+      <c r="K56">
+        <v>2022</v>
+      </c>
+      <c r="L56" t="s">
+        <v>96</v>
+      </c>
+      <c r="N56" t="s">
+        <v>100</v>
+      </c>
+      <c r="O56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57">
+        <v>7</v>
+      </c>
+      <c r="H57">
+        <v>7</v>
+      </c>
+      <c r="I57">
+        <v>100</v>
+      </c>
+      <c r="J57" t="s">
+        <v>93</v>
+      </c>
+      <c r="K57">
+        <v>2023</v>
+      </c>
+      <c r="L57" t="s">
+        <v>98</v>
+      </c>
+      <c r="N57" t="s">
+        <v>100</v>
+      </c>
+      <c r="O57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58">
+        <v>9</v>
+      </c>
+      <c r="H58">
+        <v>8.555</v>
+      </c>
+      <c r="I58">
+        <v>95</v>
+      </c>
+      <c r="J58" t="s">
+        <v>93</v>
+      </c>
+      <c r="K58">
+        <v>2023</v>
+      </c>
+      <c r="L58" t="s">
+        <v>98</v>
+      </c>
+      <c r="N58" t="s">
+        <v>100</v>
+      </c>
+      <c r="O58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" t="s">
+        <v>90</v>
+      </c>
+      <c r="G59">
+        <v>35</v>
+      </c>
+      <c r="H59">
+        <v>33.822</v>
+      </c>
+      <c r="I59">
+        <v>97</v>
+      </c>
+      <c r="J59" t="s">
+        <v>93</v>
+      </c>
+      <c r="K59">
+        <v>2023</v>
+      </c>
+      <c r="L59" t="s">
+        <v>98</v>
+      </c>
+      <c r="N59" t="s">
+        <v>100</v>
+      </c>
+      <c r="O59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" t="s">
+        <v>85</v>
+      </c>
+      <c r="G60">
+        <v>35</v>
+      </c>
+      <c r="H60">
+        <v>30.81</v>
+      </c>
+      <c r="I60">
+        <v>88</v>
+      </c>
+      <c r="J60" t="s">
+        <v>93</v>
+      </c>
+      <c r="K60">
+        <v>2023</v>
+      </c>
+      <c r="L60" t="s">
+        <v>98</v>
+      </c>
+      <c r="N60" t="s">
+        <v>100</v>
+      </c>
+      <c r="O60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" t="s">
+        <v>86</v>
+      </c>
+      <c r="G61">
+        <v>9</v>
+      </c>
+      <c r="H61">
+        <v>7.85</v>
+      </c>
+      <c r="I61">
+        <v>87</v>
+      </c>
+      <c r="J61" t="s">
+        <v>93</v>
+      </c>
+      <c r="K61">
+        <v>2023</v>
+      </c>
+      <c r="L61" t="s">
+        <v>98</v>
+      </c>
+      <c r="N61" t="s">
+        <v>100</v>
+      </c>
+      <c r="O61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" t="s">
+        <v>87</v>
+      </c>
+      <c r="G62">
+        <v>5</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>20</v>
+      </c>
+      <c r="J62" t="s">
+        <v>95</v>
+      </c>
+      <c r="K62">
+        <v>2023</v>
+      </c>
+      <c r="L62" t="s">
+        <v>98</v>
+      </c>
+      <c r="N62" t="s">
+        <v>100</v>
+      </c>
+      <c r="O62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63">
+        <v>100</v>
+      </c>
+      <c r="H63">
+        <v>89.03700000000001</v>
+      </c>
+      <c r="I63">
+        <v>89</v>
+      </c>
+      <c r="J63" t="s">
+        <v>93</v>
+      </c>
+      <c r="K63">
+        <v>2023</v>
+      </c>
+      <c r="L63" t="s">
+        <v>98</v>
+      </c>
+      <c r="N63" t="s">
+        <v>100</v>
+      </c>
+      <c r="O63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>91</v>
+      </c>
+      <c r="G64">
+        <v>5</v>
+      </c>
+      <c r="H64">
+        <v>20</v>
+      </c>
+      <c r="K64">
+        <v>2024</v>
+      </c>
+      <c r="L64" t="s">
+        <v>99</v>
+      </c>
+      <c r="N64" t="s">
+        <v>100</v>
+      </c>
+      <c r="O64" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>